<commit_message>
Now have working Python scripts for both directions : XML to Excel and Excel to XML. Also have provided sample files. Scripts have not been tested against a wide array of Archi models, so updates may be required in future.
</commit_message>
<xml_diff>
--- a/application-business-functions.xlsx
+++ b/application-business-functions.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abcoa\OneDrive\Projects\archi-xml-excel-converter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="159344FC5A44A3D6DFA585D775B87735E5455428" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{1E09C87B-65E1-4D9C-92DA-A671BF400929}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="620" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="elements" sheetId="2" r:id="rId2"/>
     <sheet name="relationships" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -133,8 +139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,10 +192,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -197,6 +206,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -243,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +292,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +344,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,14 +537,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -513,14 +570,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -534,21 +599,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -559,7 +624,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -570,21 +635,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -595,7 +660,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -612,14 +677,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="38.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -633,7 +705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -647,7 +719,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -661,7 +733,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -675,7 +747,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -689,7 +761,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -703,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>

</xml_diff>